<commit_message>
ode review checklist updated
</commit_message>
<xml_diff>
--- a/doc/Code_Review_Checklist_Group1.xlsx
+++ b/doc/Code_Review_Checklist_Group1.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dugun\Desktop\Final Documents Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B6EC71C-C7C8-428D-AA68-891A5C32F855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15D2023-B25C-44CF-AEFE-CAC585DAF999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
+    <workbookView xWindow="1032" yWindow="-108" windowWidth="22116" windowHeight="13176" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
     <sheet name="Code_Review_Checklist" sheetId="2" r:id="rId2"/>
     <sheet name="Revision History" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -82,9 +80,6 @@
   </si>
   <si>
     <t>P VIGNESHWAR</t>
-  </si>
-  <si>
-    <t>Signlas execution</t>
   </si>
   <si>
     <t>DUGUNEPALLI SUNIL KUMAR</t>
@@ -401,6 +396,9 @@
   </si>
   <si>
     <t>https://github.com/Vigneshbkaran/LMS</t>
+  </si>
+  <si>
+    <t>Signals execution,Makefile</t>
   </si>
 </sst>
 </file>
@@ -979,96 +977,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,6 +986,96 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1101,7 +1099,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1120,6 +1117,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1293,8 +1291,8 @@
     <tableColumn id="1" xr3:uid="{222501E0-6652-458C-BA66-CE8A90480925}" name="Rev." dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B0F15079-1CE5-4272-AC27-A6D5A783EB27}" name="Date of issue" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{021FC0B6-3FDF-4EFA-B528-9746EB1E617C}" name="Author" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1610,25 +1608,25 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="8" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1636,7 +1634,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1644,45 +1642,45 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="78" t="s">
-        <v>90</v>
+      <c r="D11" s="48" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="79" t="s">
-        <v>90</v>
+      <c r="D12" s="49" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="77" t="s">
-        <v>88</v>
+      <c r="D13" s="47" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1718,20 +1716,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="B2" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
@@ -1744,12 +1742,12 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="16">
         <v>22.04</v>
@@ -1758,38 +1756,38 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="72"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="145.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60">
+      <c r="B8" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64">
         <v>-1</v>
       </c>
-      <c r="E8" s="61"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
@@ -1818,43 +1816,43 @@
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
-    </row>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
     </row>
     <row r="14" spans="2:7" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="F14" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="G14" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1862,10 +1860,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="26"/>
@@ -1876,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="26"/>
@@ -1894,24 +1892,24 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="65">
+      <c r="B18" s="54">
         <v>4</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="65">
+      <c r="B19" s="54">
         <v>5</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="29"/>
@@ -1922,43 +1920,43 @@
       <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
     </row>
     <row r="23" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D23" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="E23" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F23" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1966,10 +1964,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="26"/>
@@ -1980,34 +1978,34 @@
         <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="26"/>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="54"/>
+      <c r="B26" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="24">
         <v>3</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="26"/>
@@ -2018,10 +2016,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="26"/>
@@ -2032,10 +2030,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="26"/>
@@ -2046,10 +2044,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="26"/>
@@ -2060,34 +2058,34 @@
         <v>7</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="26"/>
       <c r="G31" s="28"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="54"/>
+      <c r="B32" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="74"/>
     </row>
     <row r="33" spans="2:7" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="24">
         <v>8</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="26"/>
@@ -2098,34 +2096,34 @@
         <v>9</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" s="27"/>
       <c r="F34" s="26"/>
       <c r="G34" s="28"/>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
+      <c r="B35" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="74"/>
     </row>
     <row r="36" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="24">
         <v>10</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="26"/>
@@ -2136,10 +2134,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="26"/>
@@ -2150,10 +2148,10 @@
         <v>12</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="26"/>
@@ -2164,10 +2162,10 @@
         <v>13</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="26"/>
@@ -2178,10 +2176,10 @@
         <v>14</v>
       </c>
       <c r="C40" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="31" t="s">
         <v>62</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>63</v>
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="26"/>
@@ -2192,10 +2190,10 @@
         <v>15</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="26"/>
@@ -2206,10 +2204,10 @@
         <v>16</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="26"/>
@@ -2220,10 +2218,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="26"/>
@@ -2234,10 +2232,10 @@
         <v>18</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44" s="26"/>
@@ -2248,10 +2246,10 @@
         <v>19</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="26"/>
@@ -2262,10 +2260,10 @@
         <v>20</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="26"/>
@@ -2276,10 +2274,10 @@
         <v>21</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="26"/>
@@ -2290,10 +2288,10 @@
         <v>22</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="26"/>
@@ -2304,10 +2302,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49" s="36"/>
       <c r="F49" s="37"/>
@@ -2322,43 +2320,43 @@
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="77"/>
+    </row>
+    <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="57"/>
-    </row>
-    <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="51"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="71"/>
     </row>
     <row r="53" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="D53" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F53" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2366,10 +2364,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
@@ -2380,10 +2378,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="32" t="s">
         <v>76</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>77</v>
       </c>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
@@ -2394,10 +2392,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
@@ -2408,10 +2406,10 @@
         <v>4</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
@@ -2422,43 +2420,43 @@
         <v>5</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
       <c r="G58" s="28"/>
     </row>
     <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="51"/>
+      <c r="B59" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="71"/>
     </row>
     <row r="60" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="E60" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F60" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2466,10 +2464,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
@@ -2480,10 +2478,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
@@ -2494,10 +2492,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
@@ -2508,19 +2506,19 @@
         <v>4</v>
       </c>
       <c r="C64" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D64" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E64" s="26" t="s">
-        <v>86</v>
-      </c>
       <c r="F64" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2557,6 +2555,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B51:G51"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="B5:C5"/>
@@ -2569,14 +2575,6 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2587,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57CE01F-9AEF-4321-A1AC-1C7E0CB99876}">
   <dimension ref="F4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2600,20 +2598,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="7" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F7" s="7" t="s">
@@ -2625,7 +2623,7 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="75" t="s">
+      <c r="I7" s="45" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -2642,11 +2640,11 @@
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="76" t="s">
-        <v>89</v>
+      <c r="I8" s="46" t="s">
+        <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2657,13 +2655,13 @@
         <v>44886</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I9" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2674,13 +2672,13 @@
         <v>44888</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I10" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2691,13 +2689,13 @@
         <v>44886</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="I11" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2708,13 +2706,13 @@
         <v>44888</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I12" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revert "ode review checklist updated"
This reverts commit 39ed0df840c0237f9ffe25621e07d5e0804f5c56.
</commit_message>
<xml_diff>
--- a/doc/Code_Review_Checklist_Group1.xlsx
+++ b/doc/Code_Review_Checklist_Group1.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dugun\Desktop\Final Documents Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15D2023-B25C-44CF-AEFE-CAC585DAF999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B6EC71C-C7C8-428D-AA68-891A5C32F855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="-108" windowWidth="22116" windowHeight="13176" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
     <sheet name="Code_Review_Checklist" sheetId="2" r:id="rId2"/>
     <sheet name="Revision History" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -80,6 +82,9 @@
   </si>
   <si>
     <t>P VIGNESHWAR</t>
+  </si>
+  <si>
+    <t>Signlas execution</t>
   </si>
   <si>
     <t>DUGUNEPALLI SUNIL KUMAR</t>
@@ -396,9 +401,6 @@
   </si>
   <si>
     <t>https://github.com/Vigneshbkaran/LMS</t>
-  </si>
-  <si>
-    <t>Signals execution,Makefile</t>
   </si>
 </sst>
 </file>
@@ -977,6 +979,96 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -986,96 +1078,6 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1099,6 +1101,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1117,7 +1120,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1291,8 +1293,8 @@
     <tableColumn id="1" xr3:uid="{222501E0-6652-458C-BA66-CE8A90480925}" name="Rev." dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B0F15079-1CE5-4272-AC27-A6D5A783EB27}" name="Date of issue" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{021FC0B6-3FDF-4EFA-B528-9746EB1E617C}" name="Author" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1608,25 +1610,25 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
     </row>
     <row r="8" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1634,7 +1636,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1642,45 +1644,45 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="48" t="s">
-        <v>89</v>
+      <c r="D11" s="78" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>89</v>
+      <c r="D12" s="79" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>87</v>
+      <c r="D13" s="77" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="48"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1716,20 +1718,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="B2" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
@@ -1742,12 +1744,12 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="59"/>
+      <c r="B5" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="70"/>
       <c r="D5" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="16">
         <v>22.04</v>
@@ -1756,38 +1758,38 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60" t="s">
+      <c r="B6" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="72"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="145.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60" t="s">
+      <c r="B7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="61"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="72"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64">
+      <c r="B8" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60">
         <v>-1</v>
       </c>
-      <c r="E8" s="65"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
@@ -1816,43 +1818,43 @@
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68"/>
+      <c r="B12" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
     </row>
     <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="69" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="71"/>
+      <c r="B13" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
     </row>
     <row r="14" spans="2:7" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1860,10 +1862,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="26"/>
@@ -1874,10 +1876,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="26"/>
@@ -1892,24 +1894,24 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="54">
+      <c r="B18" s="65">
         <v>4</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67"/>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="54">
+      <c r="B19" s="65">
         <v>5</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="56"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="29"/>
@@ -1920,43 +1922,43 @@
       <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="71"/>
+      <c r="B21" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
     </row>
     <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="74"/>
+      <c r="B22" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="54"/>
     </row>
     <row r="23" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1964,10 +1966,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="26"/>
@@ -1978,34 +1980,34 @@
         <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="26"/>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="74"/>
+      <c r="B26" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="54"/>
     </row>
     <row r="27" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="24">
         <v>3</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="26"/>
@@ -2016,10 +2018,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="26"/>
@@ -2030,10 +2032,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="26"/>
@@ -2044,10 +2046,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="26"/>
@@ -2058,34 +2060,34 @@
         <v>7</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="26"/>
       <c r="G31" s="28"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="74"/>
+      <c r="B32" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="54"/>
     </row>
     <row r="33" spans="2:7" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="24">
         <v>8</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="26"/>
@@ -2096,34 +2098,34 @@
         <v>9</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E34" s="27"/>
       <c r="F34" s="26"/>
       <c r="G34" s="28"/>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="72" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="74"/>
+      <c r="B35" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="54"/>
     </row>
     <row r="36" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="24">
         <v>10</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="26"/>
@@ -2134,10 +2136,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="26"/>
@@ -2148,10 +2150,10 @@
         <v>12</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="26"/>
@@ -2162,10 +2164,10 @@
         <v>13</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="26"/>
@@ -2176,10 +2178,10 @@
         <v>14</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="26"/>
@@ -2190,10 +2192,10 @@
         <v>15</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="26"/>
@@ -2204,10 +2206,10 @@
         <v>16</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="26"/>
@@ -2218,10 +2220,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="26"/>
@@ -2232,10 +2234,10 @@
         <v>18</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44" s="26"/>
@@ -2246,10 +2248,10 @@
         <v>19</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="26"/>
@@ -2260,10 +2262,10 @@
         <v>20</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="26"/>
@@ -2274,10 +2276,10 @@
         <v>21</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="26"/>
@@ -2288,10 +2290,10 @@
         <v>22</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="26"/>
@@ -2302,10 +2304,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E49" s="36"/>
       <c r="F49" s="37"/>
@@ -2320,43 +2322,43 @@
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="76"/>
-      <c r="D51" s="76"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="76"/>
-      <c r="G51" s="77"/>
+      <c r="B51" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="57"/>
     </row>
     <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="71"/>
+      <c r="B52" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="51"/>
     </row>
     <row r="53" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2364,10 +2366,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
@@ -2378,10 +2380,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
@@ -2392,10 +2394,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
@@ -2406,10 +2408,10 @@
         <v>4</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
@@ -2420,43 +2422,43 @@
         <v>5</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
       <c r="G58" s="28"/>
     </row>
     <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="70"/>
-      <c r="D59" s="70"/>
-      <c r="E59" s="70"/>
-      <c r="F59" s="70"/>
-      <c r="G59" s="71"/>
+      <c r="B59" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="51"/>
     </row>
     <row r="60" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2464,10 +2466,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
@@ -2478,10 +2480,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
@@ -2492,10 +2494,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
@@ -2506,19 +2508,19 @@
         <v>4</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2555,14 +2557,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B51:G51"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="B5:C5"/>
@@ -2575,6 +2569,14 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2585,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57CE01F-9AEF-4321-A1AC-1C7E0CB99876}">
   <dimension ref="F4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,20 +2600,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="5" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="7" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F7" s="7" t="s">
@@ -2623,7 +2625,7 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="I7" s="75" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -2640,11 +2642,11 @@
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="46" t="s">
-        <v>88</v>
+      <c r="I8" s="76" t="s">
+        <v>89</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2655,13 +2657,13 @@
         <v>44886</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="46" t="s">
-        <v>88</v>
+        <v>16</v>
+      </c>
+      <c r="I9" s="76" t="s">
+        <v>89</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2672,13 +2674,13 @@
         <v>44888</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="I10" s="76" t="s">
+        <v>89</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2689,13 +2691,13 @@
         <v>44886</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="46" t="s">
-        <v>88</v>
+        <v>20</v>
+      </c>
+      <c r="I11" s="76" t="s">
+        <v>89</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2706,13 +2708,13 @@
         <v>44888</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>88</v>
+        <v>22</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>89</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
code review checklist updated
</commit_message>
<xml_diff>
--- a/doc/Code_Review_Checklist_Group1.xlsx
+++ b/doc/Code_Review_Checklist_Group1.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dugun\Desktop\Final Documents Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B6EC71C-C7C8-428D-AA68-891A5C32F855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15D2023-B25C-44CF-AEFE-CAC585DAF999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
+    <workbookView xWindow="1032" yWindow="-108" windowWidth="22116" windowHeight="13176" activeTab="2" xr2:uid="{32AA44BC-0B1F-4A2C-BA7A-C38CCDB98908}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
     <sheet name="Code_Review_Checklist" sheetId="2" r:id="rId2"/>
     <sheet name="Revision History" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -82,9 +80,6 @@
   </si>
   <si>
     <t>P VIGNESHWAR</t>
-  </si>
-  <si>
-    <t>Signlas execution</t>
   </si>
   <si>
     <t>DUGUNEPALLI SUNIL KUMAR</t>
@@ -401,6 +396,9 @@
   </si>
   <si>
     <t>https://github.com/Vigneshbkaran/LMS</t>
+  </si>
+  <si>
+    <t>Signals execution,Makefile</t>
   </si>
 </sst>
 </file>
@@ -979,96 +977,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,6 +986,96 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1101,7 +1099,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1120,6 +1117,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1293,8 +1291,8 @@
     <tableColumn id="1" xr3:uid="{222501E0-6652-458C-BA66-CE8A90480925}" name="Rev." dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B0F15079-1CE5-4272-AC27-A6D5A783EB27}" name="Date of issue" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{021FC0B6-3FDF-4EFA-B528-9746EB1E617C}" name="Author" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B43E3035-A5DB-4DF9-B2E3-3E282F304357}" name="Approver" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00754038-E5E9-48BE-AB51-6730EEF51BDC}" name="Description of Change" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1610,25 +1608,25 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="8" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1636,7 +1634,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1644,45 +1642,45 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="78" t="s">
-        <v>90</v>
+      <c r="D11" s="48" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="79" t="s">
-        <v>90</v>
+      <c r="D12" s="49" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="77" t="s">
-        <v>88</v>
+      <c r="D13" s="47" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1718,20 +1716,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="B2" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
@@ -1744,12 +1742,12 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="16">
         <v>22.04</v>
@@ -1758,38 +1756,38 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="72"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="145.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60">
+      <c r="B8" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64">
         <v>-1</v>
       </c>
-      <c r="E8" s="61"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
@@ -1818,43 +1816,43 @@
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
-    </row>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
     </row>
     <row r="14" spans="2:7" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="F14" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="G14" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1862,10 +1860,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="26"/>
@@ -1876,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="26"/>
@@ -1894,24 +1892,24 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="65">
+      <c r="B18" s="54">
         <v>4</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="65">
+      <c r="B19" s="54">
         <v>5</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="29"/>
@@ -1922,43 +1920,43 @@
       <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
     </row>
     <row r="23" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D23" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="E23" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F23" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1966,10 +1964,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="26"/>
@@ -1980,34 +1978,34 @@
         <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="26"/>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="54"/>
+      <c r="B26" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="24">
         <v>3</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="26"/>
@@ -2018,10 +2016,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="26"/>
@@ -2032,10 +2030,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="26"/>
@@ -2046,10 +2044,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="26"/>
@@ -2060,34 +2058,34 @@
         <v>7</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="26"/>
       <c r="G31" s="28"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="54"/>
+      <c r="B32" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="74"/>
     </row>
     <row r="33" spans="2:7" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="24">
         <v>8</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="26"/>
@@ -2098,34 +2096,34 @@
         <v>9</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" s="27"/>
       <c r="F34" s="26"/>
       <c r="G34" s="28"/>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
+      <c r="B35" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="74"/>
     </row>
     <row r="36" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="24">
         <v>10</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="26"/>
@@ -2136,10 +2134,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="26"/>
@@ -2150,10 +2148,10 @@
         <v>12</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="26"/>
@@ -2164,10 +2162,10 @@
         <v>13</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="26"/>
@@ -2178,10 +2176,10 @@
         <v>14</v>
       </c>
       <c r="C40" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="31" t="s">
         <v>62</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>63</v>
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="26"/>
@@ -2192,10 +2190,10 @@
         <v>15</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="26"/>
@@ -2206,10 +2204,10 @@
         <v>16</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="26"/>
@@ -2220,10 +2218,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="26"/>
@@ -2234,10 +2232,10 @@
         <v>18</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44" s="26"/>
@@ -2248,10 +2246,10 @@
         <v>19</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="26"/>
@@ -2262,10 +2260,10 @@
         <v>20</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="26"/>
@@ -2276,10 +2274,10 @@
         <v>21</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="26"/>
@@ -2290,10 +2288,10 @@
         <v>22</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="26"/>
@@ -2304,10 +2302,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49" s="36"/>
       <c r="F49" s="37"/>
@@ -2322,43 +2320,43 @@
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="77"/>
+    </row>
+    <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="57"/>
-    </row>
-    <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="51"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="71"/>
     </row>
     <row r="53" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="D53" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F53" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2366,10 +2364,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
@@ -2380,10 +2378,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="32" t="s">
         <v>76</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>77</v>
       </c>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
@@ -2394,10 +2392,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
@@ -2408,10 +2406,10 @@
         <v>4</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
@@ -2422,43 +2420,43 @@
         <v>5</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
       <c r="G58" s="28"/>
     </row>
     <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="51"/>
+      <c r="B59" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="71"/>
     </row>
     <row r="60" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="E60" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="F60" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -2466,10 +2464,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
@@ -2480,10 +2478,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
@@ -2494,10 +2492,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
@@ -2508,19 +2506,19 @@
         <v>4</v>
       </c>
       <c r="C64" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D64" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E64" s="26" t="s">
-        <v>86</v>
-      </c>
       <c r="F64" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2557,6 +2555,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B51:G51"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="B5:C5"/>
@@ -2569,14 +2575,6 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2587,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57CE01F-9AEF-4321-A1AC-1C7E0CB99876}">
   <dimension ref="F4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2600,20 +2598,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="7" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F7" s="7" t="s">
@@ -2625,7 +2623,7 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="75" t="s">
+      <c r="I7" s="45" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -2642,11 +2640,11 @@
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="76" t="s">
-        <v>89</v>
+      <c r="I8" s="46" t="s">
+        <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2657,13 +2655,13 @@
         <v>44886</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I9" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2674,13 +2672,13 @@
         <v>44888</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I10" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2691,13 +2689,13 @@
         <v>44886</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="I11" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="6:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -2708,13 +2706,13 @@
         <v>44888</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I12" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.3">

</xml_diff>